<commit_message>
se crean mas signos vitales
</commit_message>
<xml_diff>
--- a/recursos.xlsx
+++ b/recursos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Downloads\connectathon-2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977F6E2B-97AE-495C-888E-7AD01581330C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED932C03-1F3A-44EB-9DC0-1301307B59C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86D818FF-B0C9-44B0-8F32-14A2A2DD0110}"/>
+    <workbookView xWindow="-24154" yWindow="977" windowWidth="24267" windowHeight="13022" xr2:uid="{86D818FF-B0C9-44B0-8F32-14A2A2DD0110}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>de3629e7-45aa-4bfe-aaba-e9872062684c</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>PA Diastolica</t>
+  </si>
+  <si>
+    <t>temperatura</t>
+  </si>
+  <si>
+    <t>Frecuencia Respiratoria</t>
+  </si>
+  <si>
+    <t>Saturación O2</t>
+  </si>
+  <si>
+    <t>Escala de Dolor (EVA)</t>
   </si>
 </sst>
 </file>
@@ -531,10 +543,10 @@
   <dimension ref="D4:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="25.21875" customWidth="1"/>
     <col min="5" max="5" width="58.44140625" customWidth="1"/>
@@ -542,7 +554,7 @@
     <col min="11" max="11" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>20</v>
       </c>
@@ -559,7 +571,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>21</v>
       </c>
@@ -570,7 +582,7 @@
         <v>4634</v>
       </c>
     </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
@@ -581,7 +593,7 @@
         <v>4408</v>
       </c>
     </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
@@ -592,7 +604,7 @@
         <v>4474</v>
       </c>
     </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
@@ -600,7 +612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D9" s="3" t="s">
         <v>27</v>
       </c>
@@ -608,7 +620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D10" s="3" t="s">
         <v>28</v>
       </c>
@@ -616,7 +628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D11" s="3" t="s">
         <v>29</v>
       </c>
@@ -624,62 +636,74 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D12" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D13" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D14" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D15" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E23" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
don paolo se le cae la pizza por el *
</commit_message>
<xml_diff>
--- a/recursos.xlsx
+++ b/recursos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Downloads\connectathon-2026\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Downloads\connectathon 2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED932C03-1F3A-44EB-9DC0-1301307B59C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA820760-CB62-41E7-BFB3-3E4AF955A846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24154" yWindow="977" windowWidth="24267" windowHeight="13022" xr2:uid="{86D818FF-B0C9-44B0-8F32-14A2A2DD0110}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86D818FF-B0C9-44B0-8F32-14A2A2DD0110}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>de3629e7-45aa-4bfe-aaba-e9872062684c</t>
   </si>
@@ -138,6 +138,24 @@
   </si>
   <si>
     <t>Escala de Dolor (EVA)</t>
+  </si>
+  <si>
+    <t>Med General</t>
+  </si>
+  <si>
+    <t>Med Cirjano</t>
+  </si>
+  <si>
+    <t>prot</t>
+  </si>
+  <si>
+    <t>bioq</t>
+  </si>
+  <si>
+    <t>orina</t>
+  </si>
+  <si>
+    <t>abdominal</t>
   </si>
 </sst>
 </file>
@@ -543,10 +561,10 @@
   <dimension ref="D4:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="25.21875" customWidth="1"/>
     <col min="5" max="5" width="58.44140625" customWidth="1"/>
@@ -554,7 +572,7 @@
     <col min="11" max="11" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>20</v>
       </c>
@@ -571,7 +589,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>21</v>
       </c>
@@ -582,7 +600,7 @@
         <v>4634</v>
       </c>
     </row>
-    <row r="6" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
@@ -593,7 +611,7 @@
         <v>4408</v>
       </c>
     </row>
-    <row r="7" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
@@ -604,7 +622,7 @@
         <v>4474</v>
       </c>
     </row>
-    <row r="8" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
@@ -612,7 +630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D9" s="3" t="s">
         <v>27</v>
       </c>
@@ -620,7 +638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D10" s="3" t="s">
         <v>28</v>
       </c>
@@ -628,7 +646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D11" s="3" t="s">
         <v>29</v>
       </c>
@@ -636,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D12" s="3" t="s">
         <v>30</v>
       </c>
@@ -644,7 +662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:11" ht="15" x14ac:dyDescent="0.3">
       <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
@@ -660,7 +678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:11" ht="15" x14ac:dyDescent="0.3">
       <c r="D15" s="3" t="s">
         <v>33</v>
       </c>
@@ -668,42 +686,60 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="4:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D16" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D19" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="5:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E23" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>